<commit_message>
updated code for pdf extracted text file
</commit_message>
<xml_diff>
--- a/resources/actual_excel.xlsx
+++ b/resources/actual_excel.xlsx
@@ -19,48 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Yadav</t>
-  </si>
-  <si>
-    <t>Hello Selenium</t>
-  </si>
-  <si>
-    <t>http://www.helloselenium.com</t>
-  </si>
-  <si>
-    <t>8512888161</t>
-  </si>
-  <si>
-    <t>Abhishek</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+  <si>
+    <t>Full Name of Legal Entity</t>
+  </si>
+  <si>
+    <t>ABCD#12345</t>
+  </si>
+  <si>
+    <t>Entity/Customer Type</t>
+  </si>
+  <si>
+    <t>Australian Company</t>
+  </si>
+  <si>
+    <t>KYC (ANZ Only)</t>
+  </si>
+  <si>
+    <t>ANZ#123</t>
+  </si>
+  <si>
+    <t>Business Identifier Number</t>
+  </si>
+  <si>
+    <t>123456789</t>
   </si>
 </sst>
 </file>
@@ -126,17 +108,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
-    </xf>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,64 +395,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="7.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="15.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="18.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="33.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="22.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="26.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>